<commit_message>
files with 1900 and 1904 data base
</commit_message>
<xml_diff>
--- a/doc/paxlist/PaxList.xlsx
+++ b/doc/paxlist/PaxList.xlsx
@@ -1,8 +1,8 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="27226"/>
-  <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="28028"/>
+  <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="17460" tabRatio="500"/>
   </bookViews>
@@ -77,7 +77,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="[$-409]d\-mmm\-yy;@"/>
+    <numFmt numFmtId="164" formatCode="[$-409]d\-mmm\-yy;@"/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
@@ -128,7 +128,7 @@
   </cellStyleXfs>
   <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -464,7 +464,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C13" sqref="C13"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
@@ -489,7 +491,7 @@
     </row>
     <row r="2" spans="1:4">
       <c r="A2" s="1">
-        <v>35063</v>
+        <v>36524</v>
       </c>
       <c r="B2" t="s">
         <v>3</v>
@@ -503,7 +505,7 @@
     </row>
     <row r="3" spans="1:4">
       <c r="A3" s="1">
-        <v>34667</v>
+        <v>36128</v>
       </c>
       <c r="B3" t="s">
         <v>6</v>
@@ -517,7 +519,7 @@
     </row>
     <row r="4" spans="1:4">
       <c r="A4" s="1">
-        <v>34270</v>
+        <v>35731</v>
       </c>
       <c r="B4" t="s">
         <v>9</v>
@@ -531,7 +533,7 @@
     </row>
     <row r="5" spans="1:4">
       <c r="A5" s="1">
-        <v>33874</v>
+        <v>35335</v>
       </c>
       <c r="B5" t="s">
         <v>12</v>
@@ -545,7 +547,7 @@
     </row>
     <row r="6" spans="1:4">
       <c r="A6" s="1">
-        <v>33476</v>
+        <v>34937</v>
       </c>
       <c r="B6" t="s">
         <v>14</v>

</xml_diff>